<commit_message>
processes min/maj af by pop; handles monomorphic loci
</commit_message>
<xml_diff>
--- a/testdata.xlsx
+++ b/testdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\smussmann\Desktop\gtseqMAF\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/mussmann/local/scripts/python/gtseqMAF/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{641601B0-5E31-4508-8AD2-FDE009BABBF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AA845D3-0CC7-4D4B-A633-99A0EC4C75B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="500" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Final Genotypes" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="33">
   <si>
     <t>Sample</t>
   </si>
@@ -100,6 +100,30 @@
   </si>
   <si>
     <t>TG</t>
+  </si>
+  <si>
+    <t>pop1</t>
+  </si>
+  <si>
+    <t>pop2</t>
+  </si>
+  <si>
+    <t>pop3</t>
+  </si>
+  <si>
+    <t>Population ID</t>
+  </si>
+  <si>
+    <t>locus_05</t>
+  </si>
+  <si>
+    <t>locus_06</t>
+  </si>
+  <si>
+    <t>TA</t>
+  </si>
+  <si>
+    <t>TC</t>
   </si>
 </sst>
 </file>
@@ -423,233 +447,351 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B1048576"/>
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>14</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>15</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>18</v>
       </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2" t="s">
+        <v>21</v>
+      </c>
+      <c r="H2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
-      <c r="B3">
-        <v>0</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3" t="s">
         <v>17</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>20</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" t="s">
         <v>20</v>
       </c>
-      <c r="C4">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
         <v>18</v>
       </c>
-      <c r="E4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
+        <v>21</v>
+      </c>
+      <c r="H4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>17</v>
       </c>
-      <c r="D5">
-        <v>0</v>
-      </c>
       <c r="E5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="B6">
-        <v>0</v>
-      </c>
-      <c r="C6" t="s">
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
         <v>17</v>
       </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6">
+        <v>0</v>
+      </c>
+      <c r="G6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
         <v>16</v>
       </c>
-      <c r="C7">
-        <v>0</v>
-      </c>
-      <c r="D7" t="s">
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
         <v>24</v>
       </c>
-      <c r="E7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" t="s">
+        <v>21</v>
+      </c>
+      <c r="H7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
         <v>22</v>
       </c>
-      <c r="D8">
-        <v>0</v>
-      </c>
       <c r="E8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>8</v>
       </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="D9" t="s">
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
         <v>18</v>
       </c>
-      <c r="E9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>21</v>
+      </c>
+      <c r="H9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>9</v>
       </c>
       <c r="B10" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
         <v>20</v>
       </c>
-      <c r="C10">
-        <v>0</v>
-      </c>
       <c r="D10">
         <v>0</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>10</v>
       </c>
       <c r="B11" t="s">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
         <v>20</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>22</v>
       </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
       <c r="E11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>0</v>
+      </c>
+      <c r="G11" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" t="s">
+        <v>27</v>
+      </c>
+      <c r="C12" t="s">
         <v>20</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>22</v>
       </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
       <c r="E12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>21</v>
+      </c>
+      <c r="H12" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>12</v>
       </c>
       <c r="B13" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" t="s">
         <v>16</v>
       </c>
-      <c r="C13" t="s">
+      <c r="D13" t="s">
         <v>22</v>
       </c>
-      <c r="D13">
-        <v>0</v>
-      </c>
       <c r="E13">
         <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13" t="s">
+        <v>21</v>
+      </c>
+      <c r="H13" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>